<commit_message>
move head code to package
</commit_message>
<xml_diff>
--- a/demo/analysis/result_report.xlsx
+++ b/demo/analysis/result_report.xlsx
@@ -448,7 +448,7 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>Across all segments, a common pattern is the consumption of one to three cups of coffee per day, often structured around daily routines such as having coffee in the morning and potentially additional cups later in the day. Key differences include the male and urban segments typically consuming two to three cups daily, often linked to energy needs and specific daily routines, while the rural and female segments show a range of one to three cups, with consumption sometimes influenced by social interactions. Overall, coffee consumption appears to be a habitual part of users' daily routines, serving both functional and social purposes.</t>
+          <t>Across the different user segments, a common pattern is that most individuals consume between two to three cups of coffee per day. Specifically, males and rural residents tend to drink around two cups daily, often timing their consumption with meals or social interactions. Urban dwellers and females typically consume three cups, with a structured routine of having coffee at set times throughout the day. The key difference lies in the slight increase in consumption among urban and female segments compared to males and rural residents. Overall, the user experience suggests a habitual and somewhat patterned approach to coffee consumption, with variations influenced by gender and living environment.</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>Across all segments, a common pattern is the preference for making coffee at home, primarily due to cost-saving and the enjoyment of the brewing routine. However, convenience significantly influences the decision to purchase coffee outside, especially in urban areas and among males and females when schedules are busy. Key differences include rural users primarily making coffee at home due to impracticality of external purchases, while urban users and females often incorporate buying coffee into their daily routines as a treat or for convenience. Overall, the user experience highlights a balance between the enjoyment and cost-effectiveness of home-brewed coffee and the convenience and indulgence of buying coffee outside.</t>
+          <t>Across the user segments, a common pattern is the preference for making the first cup of coffee at home, as it is part of their morning routine. However, there is a tendency among urban and female users to buy coffee outside later in the day for convenience or as a treat. A key difference is that male users tend to buy coffee outside more frequently due to their busy schedules, while rural users predominantly make coffee at home, enjoying the brewing ritual. Overall, the user experience reflects a balance between the convenience of purchasing coffee outside and the comfort or ritual of making it at home.</t>
         </is>
       </c>
     </row>
@@ -472,7 +472,7 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>Across all segments, taste is the most important factor when choosing coffee, with a preference for good quality and specific origins such as local roasters. Price is also a common consideration, especially for those on a budget or fixed income, though some users are willing to pay more for superior taste. Convenience is emphasized in the male and urban segments, with a preference for quick and affordable options. A notable difference is the rural segment's preference for a mild flavor, while the urban and female segments show a strong tendency to support local roasters. Overall, the user experience emphasizes the importance of taste and quality, with price and convenience playing significant roles depending on individual financial situations and lifestyle preferences.</t>
+          <t>Across all user segments, taste is consistently identified as the most important factor when choosing coffee. There is also a shared interest in quality, particularly from urban and female respondents who prefer to support local roasters. Price is a significant consideration for male and rural respondents, likely due to budget constraints such as being a student or living on a fixed income. Convenience is specifically noted by male respondents as an important factor. Overall, the user experience shows a strong emphasis on taste, with varying levels of concern for price and support for local businesses depending on the demographic.</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>Common patterns across all segments suggest that coffee positively impacts energy and productivity. Both male and urban segments emphasize coffee's role in maintaining alertness and focus during long or demanding tasks. The rural and female segments highlight coffee as part of their morning routine, with an emphasis on starting the day. A shared concern across segments is moderating coffee intake to avoid jitteriness. Key differences include the urban segment's view of coffee as a necessity for hectic schedules, while the rural segment sees it more as a morning ritual. Overall, coffee is perceived as essential for enhancing productivity and managing energy levels, with its consumption being both functional and ritualistic.</t>
+          <t>The common pattern across the segments is that all interviewees believe coffee impacts their energy and productivity positively. The male, urban, and female segments emphasize that coffee significantly helps them stay focused and alert, particularly during demanding activities like exams or meetings. The rural segment, however, views coffee more as a comforting morning ritual rather than a necessity for boosting productivity. Key differences include the reliance on coffee; urban and female segments see it as essential for maintaining productivity, while the rural segment enjoys it more for leisure. Overall, coffee is perceived as a beneficial factor for energy and productivity, though its role varies from being a crucial tool for managing busy schedules to simply enhancing the morning experience.</t>
         </is>
       </c>
     </row>
@@ -496,7 +496,7 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>The synthesis of user responses across different segments highlights several common patterns and key differences. Across all segments, coffee is consistently associated with significant personal and professional experiences, often evoking emotional connections and memorable moments. Common patterns include the role of coffee in family traditions, social events, and high-pressure situations, as well as its potential to facilitate personal enjoyment and professional networking. Key differences between segments include the rural segment's emphasis on the sensory and traditional aspects of coffee consumption, such as the use of a percolator, and the urban segment's focus on coffee's role in professional settings, such as pivotal business meetings. The male and female segments both highlight coffee's emotional and experiential significance, with females specifically noting its role in intimate rituals and professional growth. Overall, the user experience with coffee is deeply intertwined with personal memories and professional development, underscoring its dual role as a comforting ritual and a catalyst for significant life events.</t>
+          <t>The user research responses reveal that coffee consumption is intertwined with both personal and professional experiences across different segments. A common pattern is that coffee plays a significant role in memorable life events, whether they are personal or professional. For the male and urban segments, coffee is associated with career-related achievements, such as acing a test or securing a major client deal. In contrast, the rural segment associates coffee with personal life, specifically a cherished daily routine with a loved one. The female segment shares a similar professional anecdote as the urban segment, highlighting the importance of coffee in networking and career progression. Overall, coffee serves as a catalyst for important life moments, offering both personal enjoyment and professional opportunities.</t>
         </is>
       </c>
     </row>

</xml_diff>